<commit_message>
More different sized networks test files
</commit_message>
<xml_diff>
--- a/test-files/graph-tests/different-sized-networks/10-genes-0-edges.xlsx
+++ b/test-files/graph-tests/different-sized-networks/10-genes-0-edges.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="28620" windowHeight="12915"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -400,12 +405,12 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,7 +445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -475,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -511,7 +516,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -546,7 +551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -581,7 +586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -616,7 +621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -651,7 +656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -686,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -721,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -756,7 +761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -793,5 +798,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>